<commit_message>
Avaluos en activos Fijos
</commit_message>
<xml_diff>
--- a/lib/Reporte_movimiento.xlsx
+++ b/lib/Reporte_movimiento.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>MOVIMIENTO</t>
   </si>
@@ -36,45 +36,6 @@
   </si>
   <si>
     <t>RESPONSABLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Se cambio FECHA DE INVENTARIO de 2012-10-12 00:00:00.000 a 2012-10-12</t>
-  </si>
-  <si>
-    <t>2024-03-25</t>
-  </si>
-  <si>
-    <t>2012-10-12 00:00:00.000</t>
-  </si>
-  <si>
-    <t>UNI</t>
-  </si>
-  <si>
-    <t>PACO PEPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Se cambio FECHA INGRESO de 2024-03-25 00:00:00.000 a 2024-03-25</t>
-  </si>
-  <si>
-    <t>2024-03-25 00:00:00.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Se cambio FECHA DE INVENTARIO de 2012-10-12 00:00:00.000 a UNI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Se cambio OBSERVACION de  a o</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Se cambio FECHA INGRESO de 1900-01-01 00:00:00.000 a 1900-01-01</t>
-  </si>
-  <si>
-    <t>1900-01-01 00:00:00.000</t>
-  </si>
-  <si>
-    <t>1900-01-01</t>
   </si>
 </sst>
 </file>
@@ -413,7 +374,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,99 +403,6 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4"/>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6"/>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>